<commit_message>
PARCIAL 12 ago 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #07 JULIO  2022/INVENTARIO ALMACEN   JULIO   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #07 JULIO  2022/INVENTARIO ALMACEN   JULIO   2022.xlsx
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="113">
   <si>
     <t>INVENTARIO ALMACEN</t>
   </si>
@@ -608,12 +608,6 @@
     <t>7.-</t>
   </si>
   <si>
-    <t>ESTA DIFERENCIA ES CONTRA INVENTARIO FISICO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esta diferencia es contra lo fisico  y registro en almacen el traspaso 371A1 </t>
-  </si>
-  <si>
     <t>Diferencia de una Entrada  no registrada por ALMACEN</t>
   </si>
   <si>
@@ -657,6 +651,15 @@
   </si>
   <si>
     <t>CHULETA DE CERDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTA DIFERENCIA ES CONTRA INVENTARIO FISICO </t>
+  </si>
+  <si>
+    <t>INVENTARIO MAL TOMADO</t>
+  </si>
+  <si>
+    <t>Esta diferencia es contra lo fisico  y registro en almacen el traspaso 371A1  NO LA REGISTRO ALMACEN</t>
   </si>
 </sst>
 </file>
@@ -1830,7 +1833,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="417">
+  <cellXfs count="425">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2693,6 +2696,73 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="11" fillId="16" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="16" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2723,69 +2793,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2828,10 +2835,24 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="16" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="16" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3157,10 +3178,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="382" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="382"/>
+      <c r="B1" s="374" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="374"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -3172,50 +3193,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="383">
+      <c r="B2" s="375">
         <v>44591</v>
       </c>
-      <c r="C2" s="384"/>
-      <c r="F2" s="385" t="s">
+      <c r="C2" s="376"/>
+      <c r="F2" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="385"/>
-      <c r="H2" s="385"/>
+      <c r="G2" s="377"/>
+      <c r="H2" s="377"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="400" t="s">
+      <c r="K2" s="392" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="400"/>
+      <c r="L2" s="392"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="386" t="s">
+      <c r="C3" s="378" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="387"/>
+      <c r="D3" s="379"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="388" t="s">
+      <c r="F3" s="380" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="389"/>
+      <c r="G3" s="381"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="390" t="s">
+      <c r="I3" s="382" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="400"/>
-      <c r="L3" s="400"/>
-      <c r="M3" s="392" t="s">
+      <c r="K3" s="392"/>
+      <c r="L3" s="392"/>
+      <c r="M3" s="384" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="393"/>
-      <c r="O3" s="394" t="s">
+      <c r="N3" s="385"/>
+      <c r="O3" s="386" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="395"/>
+      <c r="P3" s="387"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -3237,7 +3258,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="391"/>
+      <c r="I4" s="383"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -3294,8 +3315,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="396"/>
-      <c r="P5" s="397"/>
+      <c r="O5" s="388"/>
+      <c r="P5" s="389"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -3333,8 +3354,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="398"/>
-      <c r="P6" s="399"/>
+      <c r="O6" s="390"/>
+      <c r="P6" s="391"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -3417,8 +3438,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="380"/>
-      <c r="P8" s="381"/>
+      <c r="O8" s="372"/>
+      <c r="P8" s="373"/>
     </row>
     <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
@@ -3499,8 +3520,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="372"/>
-      <c r="P10" s="373"/>
+      <c r="O10" s="395"/>
+      <c r="P10" s="396"/>
       <c r="Q10" s="53"/>
       <c r="R10" s="53"/>
     </row>
@@ -3651,8 +3672,8 @@
         <f>L14+I14</f>
         <v>-34</v>
       </c>
-      <c r="O14" s="374"/>
-      <c r="P14" s="374"/>
+      <c r="O14" s="397"/>
+      <c r="P14" s="397"/>
       <c r="Q14" s="163" t="s">
         <v>47</v>
       </c>
@@ -3866,8 +3887,8 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="O19" s="375"/>
-      <c r="P19" s="375"/>
+      <c r="O19" s="398"/>
+      <c r="P19" s="398"/>
       <c r="Q19" s="163" t="s">
         <v>49</v>
       </c>
@@ -3954,8 +3975,8 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="O21" s="376"/>
-      <c r="P21" s="376"/>
+      <c r="O21" s="399"/>
+      <c r="P21" s="399"/>
       <c r="Q21" s="163" t="s">
         <v>50</v>
       </c>
@@ -3999,8 +4020,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O22" s="377"/>
-      <c r="P22" s="378"/>
+      <c r="O22" s="400"/>
+      <c r="P22" s="401"/>
       <c r="Q22" s="150"/>
       <c r="R22" s="53"/>
       <c r="S22" s="53"/>
@@ -4106,8 +4127,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O25" s="379"/>
-      <c r="P25" s="379"/>
+      <c r="O25" s="402"/>
+      <c r="P25" s="402"/>
       <c r="Q25" s="163" t="s">
         <v>51</v>
       </c>
@@ -4499,10 +4520,10 @@
     <row r="37" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="371" t="s">
+      <c r="F37" s="394" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="371"/>
+      <c r="G37" s="394"/>
       <c r="H37" s="129">
         <f>SUM(H5:H30)</f>
         <v>35456.6</v>
@@ -4531,7 +4552,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B40" s="370" t="s">
+      <c r="B40" s="393" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="155" t="s">
@@ -4552,7 +4573,7 @@
       <c r="N40" s="160"/>
     </row>
     <row r="41" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B41" s="370"/>
+      <c r="B41" s="393"/>
       <c r="C41" s="155" t="s">
         <v>48</v>
       </c>
@@ -4571,7 +4592,7 @@
       <c r="N41" s="160"/>
     </row>
     <row r="42" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="370"/>
+      <c r="B42" s="393"/>
       <c r="C42" s="155" t="s">
         <v>49</v>
       </c>
@@ -4590,7 +4611,7 @@
       <c r="N42" s="160"/>
     </row>
     <row r="43" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="370"/>
+      <c r="B43" s="393"/>
       <c r="C43" s="155" t="s">
         <v>50</v>
       </c>
@@ -4609,7 +4630,7 @@
       <c r="N43" s="160"/>
     </row>
     <row r="44" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="370"/>
+      <c r="B44" s="393"/>
       <c r="C44" s="155" t="s">
         <v>51</v>
       </c>
@@ -4628,7 +4649,7 @@
       <c r="N44" s="160"/>
     </row>
     <row r="45" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B45" s="370"/>
+      <c r="B45" s="393"/>
       <c r="C45" s="155" t="s">
         <v>54</v>
       </c>
@@ -4654,6 +4675,14 @@
     <sortCondition ref="B7:B36"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -4666,17 +4695,9 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="K2:L3"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4717,10 +4738,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="382" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="382"/>
+      <c r="B1" s="374" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="374"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -4732,50 +4753,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="383">
+      <c r="B2" s="375">
         <v>44619</v>
       </c>
-      <c r="C2" s="384"/>
-      <c r="F2" s="385" t="s">
+      <c r="C2" s="376"/>
+      <c r="F2" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="385"/>
-      <c r="H2" s="385"/>
+      <c r="G2" s="377"/>
+      <c r="H2" s="377"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="400" t="s">
+      <c r="K2" s="392" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="400"/>
+      <c r="L2" s="392"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="386" t="s">
+      <c r="C3" s="378" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="387"/>
+      <c r="D3" s="379"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="388" t="s">
+      <c r="F3" s="380" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="389"/>
+      <c r="G3" s="381"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="390" t="s">
+      <c r="I3" s="382" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="400"/>
-      <c r="L3" s="400"/>
-      <c r="M3" s="392" t="s">
+      <c r="K3" s="392"/>
+      <c r="L3" s="392"/>
+      <c r="M3" s="384" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="393"/>
-      <c r="O3" s="394" t="s">
+      <c r="N3" s="385"/>
+      <c r="O3" s="386" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="395"/>
+      <c r="P3" s="387"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -4797,7 +4818,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="391"/>
+      <c r="I4" s="383"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -4854,8 +4875,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="396"/>
-      <c r="P5" s="397"/>
+      <c r="O5" s="388"/>
+      <c r="P5" s="389"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -4893,8 +4914,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="398"/>
-      <c r="P6" s="399"/>
+      <c r="O6" s="390"/>
+      <c r="P6" s="391"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -4979,8 +5000,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="380"/>
-      <c r="P8" s="380"/>
+      <c r="O8" s="372"/>
+      <c r="P8" s="372"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -5052,8 +5073,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="372"/>
-      <c r="P10" s="372"/>
+      <c r="O10" s="395"/>
+      <c r="P10" s="395"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -5177,8 +5198,8 @@
         <f t="shared" ref="N13:N33" si="2">L13-I13</f>
         <v>0</v>
       </c>
-      <c r="O13" s="374"/>
-      <c r="P13" s="374"/>
+      <c r="O13" s="397"/>
+      <c r="P13" s="397"/>
       <c r="Q13" s="199" t="s">
         <v>64</v>
       </c>
@@ -5374,8 +5395,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O18" s="375"/>
-      <c r="P18" s="375"/>
+      <c r="O18" s="398"/>
+      <c r="P18" s="398"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
@@ -5456,8 +5477,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O20" s="376"/>
-      <c r="P20" s="376"/>
+      <c r="O20" s="399"/>
+      <c r="P20" s="399"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -5491,8 +5512,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O21" s="377"/>
-      <c r="P21" s="377"/>
+      <c r="O21" s="400"/>
+      <c r="P21" s="400"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -5600,8 +5621,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="379"/>
-      <c r="P24" s="379"/>
+      <c r="O24" s="402"/>
+      <c r="P24" s="402"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="1"/>
     </row>
@@ -6002,10 +6023,10 @@
     <row r="36" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="126"/>
       <c r="D36" s="128"/>
-      <c r="F36" s="371" t="s">
+      <c r="F36" s="394" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="371"/>
+      <c r="G36" s="394"/>
       <c r="H36" s="129">
         <f>SUM(H5:H29)</f>
         <v>22064.760000000002</v>
@@ -6043,7 +6064,7 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="370" t="s">
+      <c r="B39" s="393" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="155" t="s">
@@ -6064,7 +6085,7 @@
       <c r="N39" s="212"/>
     </row>
     <row r="40" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="370"/>
+      <c r="B40" s="393"/>
       <c r="C40" s="204"/>
       <c r="D40" s="213"/>
       <c r="E40" s="214"/>
@@ -6079,7 +6100,7 @@
       <c r="N40" s="212"/>
     </row>
     <row r="41" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="370"/>
+      <c r="B41" s="393"/>
       <c r="C41" s="201" t="s">
         <v>48</v>
       </c>
@@ -6098,7 +6119,7 @@
       <c r="N41" s="212"/>
     </row>
     <row r="42" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="401"/>
+      <c r="B42" s="403"/>
       <c r="C42" s="204"/>
       <c r="D42" s="205"/>
       <c r="E42" s="185"/>
@@ -6113,7 +6134,7 @@
       <c r="N42" s="208"/>
     </row>
     <row r="43" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="401"/>
+      <c r="B43" s="403"/>
       <c r="C43" s="204"/>
       <c r="D43" s="209"/>
       <c r="E43" s="185"/>
@@ -6128,7 +6149,7 @@
       <c r="N43" s="208"/>
     </row>
     <row r="44" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="401"/>
+      <c r="B44" s="403"/>
       <c r="C44" s="204"/>
       <c r="D44" s="210"/>
       <c r="E44" s="185"/>
@@ -6150,6 +6171,18 @@
     <sortCondition ref="B9:B16"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O8:P8"/>
     <mergeCell ref="O24:P24"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="B39:B44"/>
@@ -6158,21 +6191,9 @@
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.27559055118110237" top="0.35433070866141736" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -6210,10 +6231,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="382" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="382"/>
+      <c r="B1" s="374" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="374"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -6225,50 +6246,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="383">
+      <c r="B2" s="375">
         <v>44647</v>
       </c>
-      <c r="C2" s="384"/>
-      <c r="F2" s="385" t="s">
+      <c r="C2" s="376"/>
+      <c r="F2" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="385"/>
-      <c r="H2" s="385"/>
+      <c r="G2" s="377"/>
+      <c r="H2" s="377"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="400" t="s">
+      <c r="K2" s="392" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="400"/>
+      <c r="L2" s="392"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="386" t="s">
+      <c r="C3" s="378" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="387"/>
+      <c r="D3" s="379"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="388" t="s">
+      <c r="F3" s="380" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="389"/>
+      <c r="G3" s="381"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="390" t="s">
+      <c r="I3" s="382" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="400"/>
-      <c r="L3" s="400"/>
-      <c r="M3" s="392" t="s">
+      <c r="K3" s="392"/>
+      <c r="L3" s="392"/>
+      <c r="M3" s="384" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="393"/>
-      <c r="O3" s="394" t="s">
+      <c r="N3" s="385"/>
+      <c r="O3" s="386" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="395"/>
+      <c r="P3" s="387"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -6290,7 +6311,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="391"/>
+      <c r="I4" s="383"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -6347,8 +6368,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="396"/>
-      <c r="P5" s="397"/>
+      <c r="O5" s="388"/>
+      <c r="P5" s="389"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -6386,8 +6407,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="398"/>
-      <c r="P6" s="399"/>
+      <c r="O6" s="390"/>
+      <c r="P6" s="391"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -6472,8 +6493,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="380"/>
-      <c r="P8" s="380"/>
+      <c r="O8" s="372"/>
+      <c r="P8" s="372"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -6545,8 +6566,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="372"/>
-      <c r="P10" s="372"/>
+      <c r="O10" s="395"/>
+      <c r="P10" s="395"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -6662,8 +6683,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="374"/>
-      <c r="P13" s="374"/>
+      <c r="O13" s="397"/>
+      <c r="P13" s="397"/>
       <c r="Q13" s="187"/>
       <c r="R13" s="188"/>
       <c r="S13" s="64"/>
@@ -6853,8 +6874,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="375"/>
-      <c r="P18" s="375"/>
+      <c r="O18" s="398"/>
+      <c r="P18" s="398"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
@@ -6923,8 +6944,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="376"/>
-      <c r="P20" s="376"/>
+      <c r="O20" s="399"/>
+      <c r="P20" s="399"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -6958,8 +6979,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="377"/>
-      <c r="P21" s="377"/>
+      <c r="O21" s="400"/>
+      <c r="P21" s="400"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -7067,8 +7088,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="379"/>
-      <c r="P24" s="379"/>
+      <c r="O24" s="402"/>
+      <c r="P24" s="402"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="185"/>
     </row>
@@ -7508,10 +7529,10 @@
     <row r="37" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="371" t="s">
+      <c r="F37" s="394" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="371"/>
+      <c r="G37" s="394"/>
       <c r="H37" s="129">
         <f>SUM(H5:H29)</f>
         <v>19776.46</v>
@@ -7644,11 +7665,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:H2"/>
@@ -7656,16 +7679,14 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O8:P8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7703,10 +7724,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="382" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="382"/>
+      <c r="B1" s="374" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="374"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -7718,50 +7739,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="383">
+      <c r="B2" s="375">
         <v>44682</v>
       </c>
-      <c r="C2" s="384"/>
-      <c r="F2" s="385" t="s">
+      <c r="C2" s="376"/>
+      <c r="F2" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="385"/>
-      <c r="H2" s="385"/>
+      <c r="G2" s="377"/>
+      <c r="H2" s="377"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="400" t="s">
+      <c r="K2" s="392" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="400"/>
+      <c r="L2" s="392"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="386" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="387"/>
+      <c r="C3" s="378" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="379"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="388" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="389"/>
+      <c r="F3" s="380" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="381"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="390" t="s">
+      <c r="I3" s="382" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="400"/>
-      <c r="L3" s="400"/>
-      <c r="M3" s="392" t="s">
+      <c r="K3" s="392"/>
+      <c r="L3" s="392"/>
+      <c r="M3" s="384" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="393"/>
-      <c r="O3" s="394" t="s">
+      <c r="N3" s="385"/>
+      <c r="O3" s="386" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="395"/>
+      <c r="P3" s="387"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -7783,7 +7804,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="391"/>
+      <c r="I4" s="383"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -7840,8 +7861,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="396"/>
-      <c r="P5" s="397"/>
+      <c r="O5" s="388"/>
+      <c r="P5" s="389"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -7879,8 +7900,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="398"/>
-      <c r="P6" s="399"/>
+      <c r="O6" s="390"/>
+      <c r="P6" s="391"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -7965,8 +7986,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="380"/>
-      <c r="P8" s="380"/>
+      <c r="O8" s="372"/>
+      <c r="P8" s="372"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -8046,8 +8067,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="372"/>
-      <c r="P10" s="372"/>
+      <c r="O10" s="395"/>
+      <c r="P10" s="395"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -8163,8 +8184,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="374"/>
-      <c r="P13" s="374"/>
+      <c r="O13" s="397"/>
+      <c r="P13" s="397"/>
       <c r="Q13" s="187"/>
       <c r="R13" s="188"/>
       <c r="S13" s="64"/>
@@ -8354,8 +8375,8 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="O18" s="375"/>
-      <c r="P18" s="375"/>
+      <c r="O18" s="398"/>
+      <c r="P18" s="398"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
@@ -8440,8 +8461,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="376"/>
-      <c r="P20" s="376"/>
+      <c r="O20" s="399"/>
+      <c r="P20" s="399"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -8475,8 +8496,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="377"/>
-      <c r="P21" s="377"/>
+      <c r="O21" s="400"/>
+      <c r="P21" s="400"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -8584,8 +8605,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="379"/>
-      <c r="P24" s="379"/>
+      <c r="O24" s="402"/>
+      <c r="P24" s="402"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="185"/>
     </row>
@@ -9033,10 +9054,10 @@
     <row r="37" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="371" t="s">
+      <c r="F37" s="394" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="371"/>
+      <c r="G37" s="394"/>
       <c r="H37" s="129">
         <f>SUM(H5:H29)</f>
         <v>33269.280000000006</v>
@@ -9075,7 +9096,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="402" t="s">
+      <c r="B40" s="404" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="254" t="s">
@@ -9096,7 +9117,7 @@
       <c r="N40" s="212"/>
     </row>
     <row r="41" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="402"/>
+      <c r="B41" s="404"/>
       <c r="C41" s="204"/>
       <c r="D41" s="249"/>
       <c r="E41" s="250"/>
@@ -9175,17 +9196,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O8:P8"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -9195,9 +9205,20 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="F37:G37"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.43307086614173229" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -9235,10 +9256,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="382" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="382"/>
+      <c r="B1" s="374" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="374"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -9250,50 +9271,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="383">
+      <c r="B2" s="375">
         <v>44710</v>
       </c>
-      <c r="C2" s="384"/>
-      <c r="F2" s="385" t="s">
+      <c r="C2" s="376"/>
+      <c r="F2" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="385"/>
-      <c r="H2" s="385"/>
+      <c r="G2" s="377"/>
+      <c r="H2" s="377"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="400" t="s">
+      <c r="K2" s="392" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="400"/>
+      <c r="L2" s="392"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="386" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="387"/>
+      <c r="C3" s="378" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="379"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="388" t="s">
-        <v>105</v>
-      </c>
-      <c r="G3" s="389"/>
+      <c r="F3" s="380" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="381"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="390" t="s">
+      <c r="I3" s="382" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="400"/>
-      <c r="L3" s="400"/>
-      <c r="M3" s="392" t="s">
+      <c r="K3" s="392"/>
+      <c r="L3" s="392"/>
+      <c r="M3" s="384" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="393"/>
-      <c r="O3" s="394" t="s">
+      <c r="N3" s="385"/>
+      <c r="O3" s="386" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="395"/>
+      <c r="P3" s="387"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -9315,7 +9336,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="391"/>
+      <c r="I4" s="383"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -9372,8 +9393,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="396"/>
-      <c r="P5" s="397"/>
+      <c r="O5" s="388"/>
+      <c r="P5" s="389"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -9411,8 +9432,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="398"/>
-      <c r="P6" s="399"/>
+      <c r="O6" s="390"/>
+      <c r="P6" s="391"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -9501,8 +9522,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="380"/>
-      <c r="P8" s="380"/>
+      <c r="O8" s="372"/>
+      <c r="P8" s="372"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -9588,8 +9609,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="372"/>
-      <c r="P10" s="372"/>
+      <c r="O10" s="395"/>
+      <c r="P10" s="395"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -9705,8 +9726,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="374"/>
-      <c r="P13" s="374"/>
+      <c r="O13" s="397"/>
+      <c r="P13" s="397"/>
       <c r="Q13" s="187"/>
       <c r="R13" s="188"/>
       <c r="S13" s="64"/>
@@ -9904,8 +9925,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="375"/>
-      <c r="P18" s="375"/>
+      <c r="O18" s="398"/>
+      <c r="P18" s="398"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
@@ -9982,8 +10003,8 @@
         <f t="shared" si="1"/>
         <v>-21</v>
       </c>
-      <c r="O20" s="376"/>
-      <c r="P20" s="376"/>
+      <c r="O20" s="399"/>
+      <c r="P20" s="399"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -10017,8 +10038,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="377"/>
-      <c r="P21" s="377"/>
+      <c r="O21" s="400"/>
+      <c r="P21" s="400"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -10130,8 +10151,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="379"/>
-      <c r="P24" s="379"/>
+      <c r="O24" s="402"/>
+      <c r="P24" s="402"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="185"/>
     </row>
@@ -10592,10 +10613,10 @@
     <row r="37" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="371" t="s">
+      <c r="F37" s="394" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="371"/>
+      <c r="G37" s="394"/>
       <c r="H37" s="129">
         <f>SUM(H5:H29)</f>
         <v>41344.509999999995</v>
@@ -10634,7 +10655,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:18" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="402" t="s">
+      <c r="B40" s="404" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="254" t="s">
@@ -10655,7 +10676,7 @@
       <c r="N40" s="212"/>
     </row>
     <row r="41" spans="2:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="402"/>
+      <c r="B41" s="404"/>
       <c r="C41" s="291" t="s">
         <v>48</v>
       </c>
@@ -10674,7 +10695,7 @@
       <c r="N41" s="212"/>
     </row>
     <row r="42" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="402"/>
+      <c r="B42" s="404"/>
       <c r="C42" s="281" t="s">
         <v>48</v>
       </c>
@@ -10697,16 +10718,16 @@
       <c r="C43" s="287" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="403" t="s">
+      <c r="D43" s="405" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="404"/>
-      <c r="F43" s="404"/>
-      <c r="G43" s="404"/>
-      <c r="H43" s="404"/>
-      <c r="I43" s="404"/>
-      <c r="J43" s="404"/>
-      <c r="K43" s="405"/>
+      <c r="E43" s="406"/>
+      <c r="F43" s="406"/>
+      <c r="G43" s="406"/>
+      <c r="H43" s="406"/>
+      <c r="I43" s="406"/>
+      <c r="J43" s="406"/>
+      <c r="K43" s="407"/>
       <c r="L43" s="206"/>
       <c r="M43" s="211"/>
       <c r="N43" s="212"/>
@@ -10714,14 +10735,14 @@
     <row r="44" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="244"/>
       <c r="C44" s="204"/>
-      <c r="D44" s="406"/>
-      <c r="E44" s="407"/>
-      <c r="F44" s="407"/>
-      <c r="G44" s="407"/>
-      <c r="H44" s="407"/>
-      <c r="I44" s="407"/>
-      <c r="J44" s="407"/>
-      <c r="K44" s="408"/>
+      <c r="D44" s="408"/>
+      <c r="E44" s="409"/>
+      <c r="F44" s="409"/>
+      <c r="G44" s="409"/>
+      <c r="H44" s="409"/>
+      <c r="I44" s="409"/>
+      <c r="J44" s="409"/>
+      <c r="K44" s="410"/>
       <c r="L44" s="206"/>
       <c r="M44" s="207"/>
       <c r="N44" s="208"/>
@@ -10761,14 +10782,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D43:K44"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="F37:G37"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -10782,9 +10795,17 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O8:P8"/>
+    <mergeCell ref="D43:K44"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="F37:G37"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.11811023622047245" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -10796,8 +10817,8 @@
   </sheetPr>
   <dimension ref="B1:X47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10822,10 +10843,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="382" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="382"/>
+      <c r="B1" s="374" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="374"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -10837,50 +10858,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="383">
+      <c r="B2" s="375">
         <v>44745</v>
       </c>
-      <c r="C2" s="384"/>
-      <c r="F2" s="385" t="s">
+      <c r="C2" s="376"/>
+      <c r="F2" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="385"/>
-      <c r="H2" s="385"/>
+      <c r="G2" s="377"/>
+      <c r="H2" s="377"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="400" t="s">
+      <c r="K2" s="392" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="400"/>
+      <c r="L2" s="392"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="386" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="387"/>
+      <c r="C3" s="378" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="379"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="388" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="389"/>
+      <c r="F3" s="380" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="381"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="390" t="s">
+      <c r="I3" s="382" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="400"/>
-      <c r="L3" s="400"/>
-      <c r="M3" s="392" t="s">
+      <c r="K3" s="392"/>
+      <c r="L3" s="392"/>
+      <c r="M3" s="384" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="393"/>
-      <c r="O3" s="394" t="s">
+      <c r="N3" s="385"/>
+      <c r="O3" s="386" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="395"/>
+      <c r="P3" s="387"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -10902,7 +10923,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="391"/>
+      <c r="I4" s="383"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -10959,8 +10980,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="396"/>
-      <c r="P5" s="397"/>
+      <c r="O5" s="388"/>
+      <c r="P5" s="389"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -10998,8 +11019,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O6" s="398"/>
-      <c r="P6" s="399"/>
+      <c r="O6" s="390"/>
+      <c r="P6" s="391"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -11084,8 +11105,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O8" s="380"/>
-      <c r="P8" s="380"/>
+      <c r="O8" s="372"/>
+      <c r="P8" s="372"/>
       <c r="Q8" s="300"/>
       <c r="R8" s="185"/>
     </row>
@@ -11171,8 +11192,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="372"/>
-      <c r="P10" s="372"/>
+      <c r="O10" s="395"/>
+      <c r="P10" s="395"/>
       <c r="Q10" s="300"/>
       <c r="R10" s="185"/>
     </row>
@@ -11296,8 +11317,8 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="O13" s="374"/>
-      <c r="P13" s="374"/>
+      <c r="O13" s="397"/>
+      <c r="P13" s="397"/>
       <c r="Q13" s="331" t="s">
         <v>91</v>
       </c>
@@ -11505,8 +11526,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O18" s="375"/>
-      <c r="P18" s="375"/>
+      <c r="O18" s="398"/>
+      <c r="P18" s="398"/>
       <c r="Q18" s="333" t="s">
         <v>92</v>
       </c>
@@ -11593,8 +11614,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O20" s="414"/>
-      <c r="P20" s="414"/>
+      <c r="O20" s="416"/>
+      <c r="P20" s="416"/>
       <c r="Q20" s="308" t="s">
         <v>89</v>
       </c>
@@ -11630,8 +11651,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O21" s="377"/>
-      <c r="P21" s="377"/>
+      <c r="O21" s="400"/>
+      <c r="P21" s="400"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -11739,8 +11760,8 @@
         <f t="shared" si="3"/>
         <v>-81</v>
       </c>
-      <c r="O24" s="379"/>
-      <c r="P24" s="379"/>
+      <c r="O24" s="402"/>
+      <c r="P24" s="402"/>
       <c r="Q24" s="334" t="s">
         <v>90</v>
       </c>
@@ -11942,13 +11963,13 @@
     </row>
     <row r="30" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="344" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C30" s="96">
         <v>-2098</v>
       </c>
       <c r="D30" s="346" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E30" s="113"/>
       <c r="F30" s="96"/>
@@ -11958,7 +11979,7 @@
         <v>-2098</v>
       </c>
       <c r="I30" s="345" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J30" s="31"/>
       <c r="K30" s="83"/>
@@ -11968,12 +11989,12 @@
         <v>2098</v>
       </c>
       <c r="N30" s="349" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O30" s="350"/>
       <c r="P30" s="351"/>
       <c r="Q30" s="352" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R30" s="185"/>
     </row>
@@ -12192,10 +12213,10 @@
     <row r="37" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="371" t="s">
+      <c r="F37" s="394" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="371"/>
+      <c r="G37" s="394"/>
       <c r="H37" s="129">
         <f>SUM(H5:H29)</f>
         <v>34604.840000000004</v>
@@ -12234,7 +12255,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:18" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="411" t="s">
+      <c r="B40" s="413" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="357" t="s">
@@ -12255,26 +12276,26 @@
       <c r="N40" s="212"/>
     </row>
     <row r="41" spans="2:18" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="412"/>
+      <c r="B41" s="414"/>
       <c r="C41" s="358" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="409" t="s">
+      <c r="D41" s="411" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="409"/>
-      <c r="F41" s="409"/>
-      <c r="G41" s="409"/>
-      <c r="H41" s="409"/>
-      <c r="I41" s="409"/>
-      <c r="J41" s="409"/>
-      <c r="K41" s="409"/>
-      <c r="L41" s="409"/>
+      <c r="E41" s="411"/>
+      <c r="F41" s="411"/>
+      <c r="G41" s="411"/>
+      <c r="H41" s="411"/>
+      <c r="I41" s="411"/>
+      <c r="J41" s="411"/>
+      <c r="K41" s="411"/>
+      <c r="L41" s="411"/>
       <c r="M41" s="211"/>
       <c r="N41" s="212"/>
     </row>
     <row r="42" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="412"/>
+      <c r="B42" s="414"/>
       <c r="C42" s="359" t="s">
         <v>49</v>
       </c>
@@ -12293,31 +12314,31 @@
       <c r="N42" s="212"/>
     </row>
     <row r="43" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="412"/>
+      <c r="B43" s="414"/>
       <c r="C43" s="360" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="410" t="s">
+      <c r="D43" s="412" t="s">
         <v>88</v>
       </c>
-      <c r="E43" s="410"/>
-      <c r="F43" s="410"/>
-      <c r="G43" s="410"/>
-      <c r="H43" s="410"/>
-      <c r="I43" s="410"/>
-      <c r="J43" s="410"/>
-      <c r="K43" s="410"/>
-      <c r="L43" s="410"/>
+      <c r="E43" s="412"/>
+      <c r="F43" s="412"/>
+      <c r="G43" s="412"/>
+      <c r="H43" s="412"/>
+      <c r="I43" s="412"/>
+      <c r="J43" s="412"/>
+      <c r="K43" s="412"/>
+      <c r="L43" s="412"/>
       <c r="M43" s="211"/>
       <c r="N43" s="212"/>
     </row>
     <row r="44" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="412"/>
+      <c r="B44" s="414"/>
       <c r="C44" s="361" t="s">
         <v>51</v>
       </c>
       <c r="D44" s="356" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E44" s="326"/>
       <c r="F44" s="326"/>
@@ -12331,12 +12352,12 @@
       <c r="N44" s="208"/>
     </row>
     <row r="45" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="412"/>
+      <c r="B45" s="414"/>
       <c r="C45" s="362" t="s">
         <v>54</v>
       </c>
       <c r="D45" s="338" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="E45" s="317"/>
       <c r="F45" s="317"/>
@@ -12346,16 +12367,19 @@
       <c r="J45" s="317"/>
       <c r="K45" s="317"/>
       <c r="L45" s="339"/>
-      <c r="M45" s="207"/>
-      <c r="N45" s="208"/>
+      <c r="M45" s="419"/>
+      <c r="N45" s="420"/>
+      <c r="O45" s="421"/>
+      <c r="P45" s="422"/>
+      <c r="Q45" s="423"/>
     </row>
     <row r="46" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="412"/>
+      <c r="B46" s="414"/>
       <c r="C46" s="363" t="s">
         <v>94</v>
       </c>
       <c r="D46" s="341" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E46" s="342"/>
       <c r="F46" s="342"/>
@@ -12369,12 +12393,12 @@
       <c r="N46" s="208"/>
     </row>
     <row r="47" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="413"/>
+      <c r="B47" s="415"/>
       <c r="C47" s="364" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="355" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="D47" s="424" t="s">
+        <v>99</v>
       </c>
       <c r="E47" s="353"/>
       <c r="F47" s="353"/>
@@ -12390,6 +12414,15 @@
     <sortCondition ref="B5:B33"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="D41:L41"/>
+    <mergeCell ref="D43:L43"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -12403,18 +12436,9 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O8:P8"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="D41:L41"/>
-    <mergeCell ref="D43:L43"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -12427,7 +12451,7 @@
   <dimension ref="B1:X49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12452,10 +12476,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="382" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="382"/>
+      <c r="B1" s="374" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="374"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -12467,50 +12491,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="383">
+      <c r="B2" s="375">
         <v>44773</v>
       </c>
-      <c r="C2" s="384"/>
-      <c r="F2" s="385" t="s">
+      <c r="C2" s="376"/>
+      <c r="F2" s="377" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="385"/>
-      <c r="H2" s="385"/>
+      <c r="G2" s="377"/>
+      <c r="H2" s="377"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="400" t="s">
+      <c r="K2" s="392" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="400"/>
+      <c r="L2" s="392"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="386" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="387"/>
+      <c r="C3" s="378" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="379"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="388" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="389"/>
+      <c r="F3" s="380" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="381"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="390" t="s">
+      <c r="I3" s="382" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="400"/>
-      <c r="L3" s="400"/>
-      <c r="M3" s="392" t="s">
+      <c r="K3" s="392"/>
+      <c r="L3" s="392"/>
+      <c r="M3" s="384" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="393"/>
-      <c r="O3" s="394" t="s">
+      <c r="N3" s="385"/>
+      <c r="O3" s="386" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="395"/>
+      <c r="P3" s="387"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -12532,7 +12556,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="391"/>
+      <c r="I4" s="383"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -12589,8 +12613,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="396"/>
-      <c r="P5" s="397"/>
+      <c r="O5" s="388"/>
+      <c r="P5" s="389"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -12628,8 +12652,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="398"/>
-      <c r="P6" s="399"/>
+      <c r="O6" s="390"/>
+      <c r="P6" s="391"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -12714,8 +12738,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="380"/>
-      <c r="P8" s="380"/>
+      <c r="O8" s="372"/>
+      <c r="P8" s="372"/>
       <c r="Q8" s="300"/>
       <c r="R8" s="185"/>
     </row>
@@ -12750,11 +12774,11 @@
       <c r="L9" s="52">
         <v>110</v>
       </c>
-      <c r="M9" s="415">
+      <c r="M9" s="370">
         <f t="shared" si="1"/>
         <v>-292.90000000000009</v>
       </c>
-      <c r="N9" s="416">
+      <c r="N9" s="371">
         <f t="shared" si="1"/>
         <v>-11</v>
       </c>
@@ -12799,8 +12823,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="372"/>
-      <c r="P10" s="372"/>
+      <c r="O10" s="395"/>
+      <c r="P10" s="395"/>
       <c r="Q10" s="300"/>
       <c r="R10" s="185"/>
     </row>
@@ -12896,18 +12920,18 @@
       <c r="D13" s="140"/>
       <c r="E13" s="27"/>
       <c r="F13" s="25">
-        <v>17385.560000000001</v>
+        <v>18001.13</v>
       </c>
       <c r="G13" s="28">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="H13" s="63">
         <f t="shared" si="0"/>
-        <v>17385.560000000001</v>
+        <v>18001.13</v>
       </c>
       <c r="I13" s="47">
         <f t="shared" si="0"/>
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="J13" s="31"/>
       <c r="K13" s="51">
@@ -12918,14 +12942,14 @@
       </c>
       <c r="M13" s="220">
         <f t="shared" si="1"/>
-        <v>615.56999999999971</v>
+        <v>0</v>
       </c>
       <c r="N13" s="270">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="O13" s="374"/>
-      <c r="P13" s="374"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="397"/>
+      <c r="P13" s="397"/>
       <c r="Q13" s="187"/>
       <c r="R13" s="188"/>
       <c r="S13" s="64"/>
@@ -13046,7 +13070,7 @@
     </row>
     <row r="17" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="264" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="26"/>
@@ -13082,9 +13106,7 @@
       </c>
       <c r="O17" s="67"/>
       <c r="P17" s="173"/>
-      <c r="Q17" s="194">
-        <v>183</v>
-      </c>
+      <c r="Q17" s="194"/>
       <c r="R17" s="185"/>
       <c r="S17" s="53"/>
       <c r="T17" s="53"/>
@@ -13183,18 +13205,18 @@
       <c r="D20" s="266"/>
       <c r="E20" s="267"/>
       <c r="F20" s="265">
-        <v>1057.82</v>
+        <v>1062.3599999999999</v>
       </c>
       <c r="G20" s="175">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H20" s="268">
         <f t="shared" si="0"/>
-        <v>1057.82</v>
+        <v>1062.3599999999999</v>
       </c>
       <c r="I20" s="269">
         <f t="shared" si="0"/>
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J20" s="241"/>
       <c r="K20" s="51">
@@ -13205,14 +13227,14 @@
       </c>
       <c r="M20" s="191">
         <f t="shared" si="8"/>
-        <v>4.5399999999999636</v>
+        <v>0</v>
       </c>
       <c r="N20" s="270">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="375"/>
-      <c r="P20" s="375"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="398"/>
+      <c r="P20" s="398"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="185"/>
       <c r="S20" s="53"/>
@@ -13223,7 +13245,7 @@
         <v>83</v>
       </c>
       <c r="C21" s="25">
-        <v>280.36</v>
+        <v>279.36</v>
       </c>
       <c r="D21" s="26">
         <v>10</v>
@@ -13233,7 +13255,7 @@
       <c r="G21" s="28"/>
       <c r="H21" s="63">
         <f t="shared" si="0"/>
-        <v>280.36</v>
+        <v>279.36</v>
       </c>
       <c r="I21" s="47">
         <f t="shared" si="0"/>
@@ -13248,7 +13270,7 @@
       </c>
       <c r="M21" s="191">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="270">
         <f t="shared" si="1"/>
@@ -13269,14 +13291,14 @@
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
       <c r="F22" s="25">
-        <v>6027.27</v>
+        <v>5997.93</v>
       </c>
       <c r="G22" s="28">
         <v>236</v>
       </c>
       <c r="H22" s="63">
         <f t="shared" si="0"/>
-        <v>6027.27</v>
+        <v>5997.93</v>
       </c>
       <c r="I22" s="47">
         <f t="shared" si="0"/>
@@ -13291,14 +13313,14 @@
       </c>
       <c r="M22" s="220">
         <f t="shared" si="1"/>
-        <v>-29.290000000000873</v>
+        <v>4.9999999999272404E-2</v>
       </c>
       <c r="N22" s="270">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O22" s="376"/>
-      <c r="P22" s="376"/>
+      <c r="O22" s="399"/>
+      <c r="P22" s="399"/>
       <c r="Q22" s="187"/>
       <c r="R22" s="189"/>
       <c r="S22" s="76"/>
@@ -13332,8 +13354,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O23" s="377"/>
-      <c r="P23" s="377"/>
+      <c r="O23" s="400"/>
+      <c r="P23" s="400"/>
       <c r="Q23" s="187"/>
       <c r="R23" s="185"/>
       <c r="S23" s="53"/>
@@ -13430,20 +13452,22 @@
       <c r="K26" s="83">
         <v>1983.68</v>
       </c>
-      <c r="L26" s="52">
-        <v>66</v>
-      </c>
-      <c r="M26" s="220">
+      <c r="L26" s="417">
+        <v>68</v>
+      </c>
+      <c r="M26" s="315">
         <f>K26-H26</f>
         <v>-7.5999999999999091</v>
       </c>
-      <c r="N26" s="270">
+      <c r="N26" s="290">
         <f t="shared" si="10"/>
-        <v>-2</v>
-      </c>
-      <c r="O26" s="379"/>
-      <c r="P26" s="379"/>
-      <c r="Q26" s="187"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="402"/>
+      <c r="P26" s="402"/>
+      <c r="Q26" s="418" t="s">
+        <v>111</v>
+      </c>
       <c r="R26" s="185"/>
     </row>
     <row r="27" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -13642,7 +13666,7 @@
     </row>
     <row r="32" spans="2:20" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="367" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C32" s="96"/>
       <c r="D32" s="346"/>
@@ -13708,7 +13732,7 @@
     </row>
     <row r="34" spans="2:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="272" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="26"/>
@@ -13910,17 +13934,17 @@
     <row r="39" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="126"/>
       <c r="D39" s="128"/>
-      <c r="F39" s="371" t="s">
+      <c r="F39" s="394" t="s">
         <v>43</v>
       </c>
-      <c r="G39" s="371"/>
+      <c r="G39" s="394"/>
       <c r="H39" s="129">
         <f>SUM(H5:H31)</f>
-        <v>65492.05</v>
+        <v>66081.820000000007</v>
       </c>
       <c r="I39" s="130">
         <f>SUM(I5:I31)</f>
-        <v>2089</v>
+        <v>2095</v>
       </c>
       <c r="J39" s="131"/>
       <c r="K39" s="132">
@@ -13952,7 +13976,7 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="2:18" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="411" t="s">
+      <c r="B42" s="413" t="s">
         <v>58</v>
       </c>
       <c r="C42" s="357" t="s">
@@ -13971,24 +13995,24 @@
       <c r="N42" s="212"/>
     </row>
     <row r="43" spans="2:18" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="412"/>
+      <c r="B43" s="414"/>
       <c r="C43" s="358" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="409"/>
-      <c r="E43" s="409"/>
-      <c r="F43" s="409"/>
-      <c r="G43" s="409"/>
-      <c r="H43" s="409"/>
-      <c r="I43" s="409"/>
-      <c r="J43" s="409"/>
-      <c r="K43" s="409"/>
-      <c r="L43" s="409"/>
+      <c r="D43" s="411"/>
+      <c r="E43" s="411"/>
+      <c r="F43" s="411"/>
+      <c r="G43" s="411"/>
+      <c r="H43" s="411"/>
+      <c r="I43" s="411"/>
+      <c r="J43" s="411"/>
+      <c r="K43" s="411"/>
+      <c r="L43" s="411"/>
       <c r="M43" s="211"/>
       <c r="N43" s="212"/>
     </row>
     <row r="44" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="412"/>
+      <c r="B44" s="414"/>
       <c r="C44" s="359" t="s">
         <v>49</v>
       </c>
@@ -14005,24 +14029,24 @@
       <c r="N44" s="212"/>
     </row>
     <row r="45" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="412"/>
+      <c r="B45" s="414"/>
       <c r="C45" s="360" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="410"/>
-      <c r="E45" s="410"/>
-      <c r="F45" s="410"/>
-      <c r="G45" s="410"/>
-      <c r="H45" s="410"/>
-      <c r="I45" s="410"/>
-      <c r="J45" s="410"/>
-      <c r="K45" s="410"/>
-      <c r="L45" s="410"/>
+      <c r="D45" s="412"/>
+      <c r="E45" s="412"/>
+      <c r="F45" s="412"/>
+      <c r="G45" s="412"/>
+      <c r="H45" s="412"/>
+      <c r="I45" s="412"/>
+      <c r="J45" s="412"/>
+      <c r="K45" s="412"/>
+      <c r="L45" s="412"/>
       <c r="M45" s="211"/>
       <c r="N45" s="212"/>
     </row>
     <row r="46" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="412"/>
+      <c r="B46" s="414"/>
       <c r="C46" s="361" t="s">
         <v>51</v>
       </c>
@@ -14039,7 +14063,7 @@
       <c r="N46" s="208"/>
     </row>
     <row r="47" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="412"/>
+      <c r="B47" s="414"/>
       <c r="C47" s="362" t="s">
         <v>54</v>
       </c>
@@ -14056,7 +14080,7 @@
       <c r="N47" s="208"/>
     </row>
     <row r="48" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="412"/>
+      <c r="B48" s="414"/>
       <c r="C48" s="363" t="s">
         <v>94</v>
       </c>
@@ -14073,9 +14097,9 @@
       <c r="N48" s="208"/>
     </row>
     <row r="49" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="413"/>
+      <c r="B49" s="415"/>
       <c r="C49" s="364" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D49" s="355"/>
       <c r="E49" s="353"/>
@@ -14089,6 +14113,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B42:B49"/>
+    <mergeCell ref="D43:L43"/>
+    <mergeCell ref="D45:L45"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F39:G39"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -14102,18 +14135,9 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B42:B49"/>
-    <mergeCell ref="D43:L43"/>
-    <mergeCell ref="D45:L45"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F39:G39"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
cierre 12 Ago 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #07 JULIO  2022/INVENTARIO ALMACEN   JULIO   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #07 JULIO  2022/INVENTARIO ALMACEN   JULIO   2022.xlsx
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="115">
   <si>
     <t>INVENTARIO ALMACEN</t>
   </si>
@@ -656,10 +656,16 @@
     <t xml:space="preserve">ESTA DIFERENCIA ES CONTRA INVENTARIO FISICO </t>
   </si>
   <si>
-    <t>INVENTARIO MAL TOMADO</t>
+    <t>Esta diferencia es contra lo fisico  y registro en almacen el traspaso 371A1  NO LA REGISTRO ALMACEN</t>
   </si>
   <si>
-    <t>Esta diferencia es contra lo fisico  y registro en almacen el traspaso 371A1  NO LA REGISTRO ALMACEN</t>
+    <t>FALTANTE DE MAYO 4 CAJAS  110.42 Kg</t>
+  </si>
+  <si>
+    <t>INVENTARIO MAL TOMADO SOLO COPEARON LOS DATOS</t>
+  </si>
+  <si>
+    <t>FALTANTE EN INVENTARIO EN ALMACEN</t>
   </si>
 </sst>
 </file>
@@ -670,7 +676,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1008,6 +1014,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF660033"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -1107,7 +1121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -1828,12 +1842,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="425">
+  <cellXfs count="445">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2659,7 +2693,6 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="15" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="33" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2700,146 +2733,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="16" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="10" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2853,6 +2748,197 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="33" fillId="12" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="9" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2862,16 +2948,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FF99"/>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FF00FFFF"/>
       <color rgb="FFFF9900"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFCC99FF"/>
-      <color rgb="FFFFCCFF"/>
-      <color rgb="FF00FFFF"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF99FF99"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF660033"/>
-      <color rgb="FF66FF99"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3178,10 +3264,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="374" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="374"/>
+      <c r="B1" s="390" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="390"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -3193,50 +3279,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="375">
+      <c r="B2" s="391">
         <v>44591</v>
       </c>
-      <c r="C2" s="376"/>
-      <c r="F2" s="377" t="s">
+      <c r="C2" s="392"/>
+      <c r="F2" s="393" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="377"/>
-      <c r="H2" s="377"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="392" t="s">
+      <c r="K2" s="408" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="392"/>
+      <c r="L2" s="408"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="378" t="s">
+      <c r="C3" s="394" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="379"/>
+      <c r="D3" s="395"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="380" t="s">
+      <c r="F3" s="396" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="381"/>
+      <c r="G3" s="397"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="382" t="s">
+      <c r="I3" s="398" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="392"/>
-      <c r="L3" s="392"/>
-      <c r="M3" s="384" t="s">
+      <c r="K3" s="408"/>
+      <c r="L3" s="408"/>
+      <c r="M3" s="400" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="385"/>
-      <c r="O3" s="386" t="s">
+      <c r="N3" s="401"/>
+      <c r="O3" s="402" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="387"/>
+      <c r="P3" s="403"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -3258,7 +3344,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="383"/>
+      <c r="I4" s="399"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -3315,8 +3401,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
-      <c r="P5" s="389"/>
+      <c r="O5" s="404"/>
+      <c r="P5" s="405"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -3354,8 +3440,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="390"/>
-      <c r="P6" s="391"/>
+      <c r="O6" s="406"/>
+      <c r="P6" s="407"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -3438,8 +3524,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="372"/>
-      <c r="P8" s="373"/>
+      <c r="O8" s="388"/>
+      <c r="P8" s="389"/>
     </row>
     <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
@@ -3520,8 +3606,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="395"/>
-      <c r="P10" s="396"/>
+      <c r="O10" s="380"/>
+      <c r="P10" s="381"/>
       <c r="Q10" s="53"/>
       <c r="R10" s="53"/>
     </row>
@@ -3672,8 +3758,8 @@
         <f>L14+I14</f>
         <v>-34</v>
       </c>
-      <c r="O14" s="397"/>
-      <c r="P14" s="397"/>
+      <c r="O14" s="382"/>
+      <c r="P14" s="382"/>
       <c r="Q14" s="163" t="s">
         <v>47</v>
       </c>
@@ -3887,8 +3973,8 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="O19" s="398"/>
-      <c r="P19" s="398"/>
+      <c r="O19" s="383"/>
+      <c r="P19" s="383"/>
       <c r="Q19" s="163" t="s">
         <v>49</v>
       </c>
@@ -3975,8 +4061,8 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="O21" s="399"/>
-      <c r="P21" s="399"/>
+      <c r="O21" s="384"/>
+      <c r="P21" s="384"/>
       <c r="Q21" s="163" t="s">
         <v>50</v>
       </c>
@@ -4020,8 +4106,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O22" s="400"/>
-      <c r="P22" s="401"/>
+      <c r="O22" s="385"/>
+      <c r="P22" s="386"/>
       <c r="Q22" s="150"/>
       <c r="R22" s="53"/>
       <c r="S22" s="53"/>
@@ -4127,8 +4213,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O25" s="402"/>
-      <c r="P25" s="402"/>
+      <c r="O25" s="387"/>
+      <c r="P25" s="387"/>
       <c r="Q25" s="163" t="s">
         <v>51</v>
       </c>
@@ -4520,10 +4606,10 @@
     <row r="37" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="394" t="s">
+      <c r="F37" s="379" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="394"/>
+      <c r="G37" s="379"/>
       <c r="H37" s="129">
         <f>SUM(H5:H30)</f>
         <v>35456.6</v>
@@ -4552,7 +4638,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B40" s="393" t="s">
+      <c r="B40" s="378" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="155" t="s">
@@ -4573,7 +4659,7 @@
       <c r="N40" s="160"/>
     </row>
     <row r="41" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B41" s="393"/>
+      <c r="B41" s="378"/>
       <c r="C41" s="155" t="s">
         <v>48</v>
       </c>
@@ -4592,7 +4678,7 @@
       <c r="N41" s="160"/>
     </row>
     <row r="42" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="393"/>
+      <c r="B42" s="378"/>
       <c r="C42" s="155" t="s">
         <v>49</v>
       </c>
@@ -4611,7 +4697,7 @@
       <c r="N42" s="160"/>
     </row>
     <row r="43" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="393"/>
+      <c r="B43" s="378"/>
       <c r="C43" s="155" t="s">
         <v>50</v>
       </c>
@@ -4630,7 +4716,7 @@
       <c r="N43" s="160"/>
     </row>
     <row r="44" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="393"/>
+      <c r="B44" s="378"/>
       <c r="C44" s="155" t="s">
         <v>51</v>
       </c>
@@ -4649,7 +4735,7 @@
       <c r="N44" s="160"/>
     </row>
     <row r="45" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B45" s="393"/>
+      <c r="B45" s="378"/>
       <c r="C45" s="155" t="s">
         <v>54</v>
       </c>
@@ -4675,14 +4761,6 @@
     <sortCondition ref="B7:B36"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -4695,6 +4773,14 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="K2:L3"/>
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
@@ -4738,10 +4824,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="374" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="374"/>
+      <c r="B1" s="390" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="390"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -4753,50 +4839,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="375">
+      <c r="B2" s="391">
         <v>44619</v>
       </c>
-      <c r="C2" s="376"/>
-      <c r="F2" s="377" t="s">
+      <c r="C2" s="392"/>
+      <c r="F2" s="393" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="377"/>
-      <c r="H2" s="377"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="392" t="s">
+      <c r="K2" s="408" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="392"/>
+      <c r="L2" s="408"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="378" t="s">
+      <c r="C3" s="394" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="379"/>
+      <c r="D3" s="395"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="380" t="s">
+      <c r="F3" s="396" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="381"/>
+      <c r="G3" s="397"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="382" t="s">
+      <c r="I3" s="398" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="392"/>
-      <c r="L3" s="392"/>
-      <c r="M3" s="384" t="s">
+      <c r="K3" s="408"/>
+      <c r="L3" s="408"/>
+      <c r="M3" s="400" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="385"/>
-      <c r="O3" s="386" t="s">
+      <c r="N3" s="401"/>
+      <c r="O3" s="402" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="387"/>
+      <c r="P3" s="403"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -4818,7 +4904,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="383"/>
+      <c r="I4" s="399"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -4875,8 +4961,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
-      <c r="P5" s="389"/>
+      <c r="O5" s="404"/>
+      <c r="P5" s="405"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -4914,8 +5000,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="390"/>
-      <c r="P6" s="391"/>
+      <c r="O6" s="406"/>
+      <c r="P6" s="407"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -5000,8 +5086,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="372"/>
-      <c r="P8" s="372"/>
+      <c r="O8" s="388"/>
+      <c r="P8" s="388"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -5073,8 +5159,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="395"/>
-      <c r="P10" s="395"/>
+      <c r="O10" s="380"/>
+      <c r="P10" s="380"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -5198,8 +5284,8 @@
         <f t="shared" ref="N13:N33" si="2">L13-I13</f>
         <v>0</v>
       </c>
-      <c r="O13" s="397"/>
-      <c r="P13" s="397"/>
+      <c r="O13" s="382"/>
+      <c r="P13" s="382"/>
       <c r="Q13" s="199" t="s">
         <v>64</v>
       </c>
@@ -5395,8 +5481,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O18" s="398"/>
-      <c r="P18" s="398"/>
+      <c r="O18" s="383"/>
+      <c r="P18" s="383"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
@@ -5477,8 +5563,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O20" s="399"/>
-      <c r="P20" s="399"/>
+      <c r="O20" s="384"/>
+      <c r="P20" s="384"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -5512,8 +5598,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O21" s="400"/>
-      <c r="P21" s="400"/>
+      <c r="O21" s="385"/>
+      <c r="P21" s="385"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -5621,8 +5707,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="402"/>
-      <c r="P24" s="402"/>
+      <c r="O24" s="387"/>
+      <c r="P24" s="387"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="1"/>
     </row>
@@ -6023,10 +6109,10 @@
     <row r="36" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="126"/>
       <c r="D36" s="128"/>
-      <c r="F36" s="394" t="s">
+      <c r="F36" s="379" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="394"/>
+      <c r="G36" s="379"/>
       <c r="H36" s="129">
         <f>SUM(H5:H29)</f>
         <v>22064.760000000002</v>
@@ -6064,7 +6150,7 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="393" t="s">
+      <c r="B39" s="378" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="155" t="s">
@@ -6085,7 +6171,7 @@
       <c r="N39" s="212"/>
     </row>
     <row r="40" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="393"/>
+      <c r="B40" s="378"/>
       <c r="C40" s="204"/>
       <c r="D40" s="213"/>
       <c r="E40" s="214"/>
@@ -6100,7 +6186,7 @@
       <c r="N40" s="212"/>
     </row>
     <row r="41" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="393"/>
+      <c r="B41" s="378"/>
       <c r="C41" s="201" t="s">
         <v>48</v>
       </c>
@@ -6119,7 +6205,7 @@
       <c r="N41" s="212"/>
     </row>
     <row r="42" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="403"/>
+      <c r="B42" s="409"/>
       <c r="C42" s="204"/>
       <c r="D42" s="205"/>
       <c r="E42" s="185"/>
@@ -6134,7 +6220,7 @@
       <c r="N42" s="208"/>
     </row>
     <row r="43" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="403"/>
+      <c r="B43" s="409"/>
       <c r="C43" s="204"/>
       <c r="D43" s="209"/>
       <c r="E43" s="185"/>
@@ -6149,7 +6235,7 @@
       <c r="N43" s="208"/>
     </row>
     <row r="44" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="403"/>
+      <c r="B44" s="409"/>
       <c r="C44" s="204"/>
       <c r="D44" s="210"/>
       <c r="E44" s="185"/>
@@ -6171,18 +6257,6 @@
     <sortCondition ref="B9:B16"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O8:P8"/>
     <mergeCell ref="O24:P24"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="B39:B44"/>
@@ -6191,6 +6265,18 @@
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.27559055118110237" top="0.35433070866141736" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
@@ -6231,10 +6317,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="374" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="374"/>
+      <c r="B1" s="390" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="390"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -6246,50 +6332,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="375">
+      <c r="B2" s="391">
         <v>44647</v>
       </c>
-      <c r="C2" s="376"/>
-      <c r="F2" s="377" t="s">
+      <c r="C2" s="392"/>
+      <c r="F2" s="393" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="377"/>
-      <c r="H2" s="377"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="392" t="s">
+      <c r="K2" s="408" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="392"/>
+      <c r="L2" s="408"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="378" t="s">
+      <c r="C3" s="394" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="379"/>
+      <c r="D3" s="395"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="380" t="s">
+      <c r="F3" s="396" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="381"/>
+      <c r="G3" s="397"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="382" t="s">
+      <c r="I3" s="398" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="392"/>
-      <c r="L3" s="392"/>
-      <c r="M3" s="384" t="s">
+      <c r="K3" s="408"/>
+      <c r="L3" s="408"/>
+      <c r="M3" s="400" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="385"/>
-      <c r="O3" s="386" t="s">
+      <c r="N3" s="401"/>
+      <c r="O3" s="402" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="387"/>
+      <c r="P3" s="403"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -6311,7 +6397,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="383"/>
+      <c r="I4" s="399"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -6368,8 +6454,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
-      <c r="P5" s="389"/>
+      <c r="O5" s="404"/>
+      <c r="P5" s="405"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -6407,8 +6493,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="390"/>
-      <c r="P6" s="391"/>
+      <c r="O6" s="406"/>
+      <c r="P6" s="407"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -6493,8 +6579,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="372"/>
-      <c r="P8" s="372"/>
+      <c r="O8" s="388"/>
+      <c r="P8" s="388"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -6566,8 +6652,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="395"/>
-      <c r="P10" s="395"/>
+      <c r="O10" s="380"/>
+      <c r="P10" s="380"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -6683,8 +6769,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="397"/>
-      <c r="P13" s="397"/>
+      <c r="O13" s="382"/>
+      <c r="P13" s="382"/>
       <c r="Q13" s="187"/>
       <c r="R13" s="188"/>
       <c r="S13" s="64"/>
@@ -6874,8 +6960,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="398"/>
-      <c r="P18" s="398"/>
+      <c r="O18" s="383"/>
+      <c r="P18" s="383"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
@@ -6944,8 +7030,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="399"/>
-      <c r="P20" s="399"/>
+      <c r="O20" s="384"/>
+      <c r="P20" s="384"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -6979,8 +7065,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="400"/>
-      <c r="P21" s="400"/>
+      <c r="O21" s="385"/>
+      <c r="P21" s="385"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -7088,8 +7174,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="402"/>
-      <c r="P24" s="402"/>
+      <c r="O24" s="387"/>
+      <c r="P24" s="387"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="185"/>
     </row>
@@ -7529,10 +7615,10 @@
     <row r="37" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="394" t="s">
+      <c r="F37" s="379" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="394"/>
+      <c r="G37" s="379"/>
       <c r="H37" s="129">
         <f>SUM(H5:H29)</f>
         <v>19776.46</v>
@@ -7665,6 +7751,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="O24:P24"/>
@@ -7672,18 +7770,6 @@
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="O18:P18"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O8:P8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
@@ -7724,10 +7810,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="374" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="374"/>
+      <c r="B1" s="390" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="390"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -7739,50 +7825,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="375">
+      <c r="B2" s="391">
         <v>44682</v>
       </c>
-      <c r="C2" s="376"/>
-      <c r="F2" s="377" t="s">
+      <c r="C2" s="392"/>
+      <c r="F2" s="393" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="377"/>
-      <c r="H2" s="377"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="392" t="s">
+      <c r="K2" s="408" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="392"/>
+      <c r="L2" s="408"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="378" t="s">
+      <c r="C3" s="394" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="379"/>
+      <c r="D3" s="395"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="380" t="s">
+      <c r="F3" s="396" t="s">
         <v>101</v>
       </c>
-      <c r="G3" s="381"/>
+      <c r="G3" s="397"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="382" t="s">
+      <c r="I3" s="398" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="392"/>
-      <c r="L3" s="392"/>
-      <c r="M3" s="384" t="s">
+      <c r="K3" s="408"/>
+      <c r="L3" s="408"/>
+      <c r="M3" s="400" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="385"/>
-      <c r="O3" s="386" t="s">
+      <c r="N3" s="401"/>
+      <c r="O3" s="402" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="387"/>
+      <c r="P3" s="403"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -7804,7 +7890,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="383"/>
+      <c r="I4" s="399"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -7861,8 +7947,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
-      <c r="P5" s="389"/>
+      <c r="O5" s="404"/>
+      <c r="P5" s="405"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -7900,8 +7986,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="390"/>
-      <c r="P6" s="391"/>
+      <c r="O6" s="406"/>
+      <c r="P6" s="407"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -7986,8 +8072,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="372"/>
-      <c r="P8" s="372"/>
+      <c r="O8" s="388"/>
+      <c r="P8" s="388"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -8067,8 +8153,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="395"/>
-      <c r="P10" s="395"/>
+      <c r="O10" s="380"/>
+      <c r="P10" s="380"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -8184,8 +8270,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="397"/>
-      <c r="P13" s="397"/>
+      <c r="O13" s="382"/>
+      <c r="P13" s="382"/>
       <c r="Q13" s="187"/>
       <c r="R13" s="188"/>
       <c r="S13" s="64"/>
@@ -8375,8 +8461,8 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="O18" s="398"/>
-      <c r="P18" s="398"/>
+      <c r="O18" s="383"/>
+      <c r="P18" s="383"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
@@ -8461,8 +8547,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="399"/>
-      <c r="P20" s="399"/>
+      <c r="O20" s="384"/>
+      <c r="P20" s="384"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -8496,8 +8582,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="400"/>
-      <c r="P21" s="400"/>
+      <c r="O21" s="385"/>
+      <c r="P21" s="385"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -8605,8 +8691,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="402"/>
-      <c r="P24" s="402"/>
+      <c r="O24" s="387"/>
+      <c r="P24" s="387"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="185"/>
     </row>
@@ -9054,10 +9140,10 @@
     <row r="37" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="394" t="s">
+      <c r="F37" s="379" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="394"/>
+      <c r="G37" s="379"/>
       <c r="H37" s="129">
         <f>SUM(H5:H29)</f>
         <v>33269.280000000006</v>
@@ -9096,7 +9182,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="404" t="s">
+      <c r="B40" s="410" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="254" t="s">
@@ -9117,7 +9203,7 @@
       <c r="N40" s="212"/>
     </row>
     <row r="41" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="404"/>
+      <c r="B41" s="410"/>
       <c r="C41" s="204"/>
       <c r="D41" s="249"/>
       <c r="E41" s="250"/>
@@ -9196,6 +9282,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O8:P8"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -9205,17 +9302,6 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="F37:G37"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.43307086614173229" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
@@ -9256,10 +9342,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="374" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="374"/>
+      <c r="B1" s="390" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="390"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -9271,50 +9357,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="375">
+      <c r="B2" s="391">
         <v>44710</v>
       </c>
-      <c r="C2" s="376"/>
-      <c r="F2" s="377" t="s">
+      <c r="C2" s="392"/>
+      <c r="F2" s="393" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="377"/>
-      <c r="H2" s="377"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="392" t="s">
+      <c r="K2" s="408" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="392"/>
+      <c r="L2" s="408"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="378" t="s">
+      <c r="C3" s="394" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="379"/>
+      <c r="D3" s="395"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="380" t="s">
+      <c r="F3" s="396" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="381"/>
+      <c r="G3" s="397"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="382" t="s">
+      <c r="I3" s="398" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="392"/>
-      <c r="L3" s="392"/>
-      <c r="M3" s="384" t="s">
+      <c r="K3" s="408"/>
+      <c r="L3" s="408"/>
+      <c r="M3" s="400" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="385"/>
-      <c r="O3" s="386" t="s">
+      <c r="N3" s="401"/>
+      <c r="O3" s="402" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="387"/>
+      <c r="P3" s="403"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -9336,7 +9422,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="383"/>
+      <c r="I4" s="399"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -9393,8 +9479,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
-      <c r="P5" s="389"/>
+      <c r="O5" s="404"/>
+      <c r="P5" s="405"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -9432,8 +9518,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="390"/>
-      <c r="P6" s="391"/>
+      <c r="O6" s="406"/>
+      <c r="P6" s="407"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -9522,8 +9608,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="372"/>
-      <c r="P8" s="372"/>
+      <c r="O8" s="388"/>
+      <c r="P8" s="388"/>
       <c r="Q8" s="193"/>
       <c r="R8" s="1"/>
     </row>
@@ -9609,8 +9695,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="395"/>
-      <c r="P10" s="395"/>
+      <c r="O10" s="380"/>
+      <c r="P10" s="380"/>
       <c r="Q10" s="193"/>
       <c r="R10" s="185"/>
     </row>
@@ -9726,8 +9812,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="397"/>
-      <c r="P13" s="397"/>
+      <c r="O13" s="382"/>
+      <c r="P13" s="382"/>
       <c r="Q13" s="187"/>
       <c r="R13" s="188"/>
       <c r="S13" s="64"/>
@@ -9925,8 +10011,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="398"/>
-      <c r="P18" s="398"/>
+      <c r="O18" s="383"/>
+      <c r="P18" s="383"/>
       <c r="Q18" s="187"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
@@ -10003,8 +10089,8 @@
         <f t="shared" si="1"/>
         <v>-21</v>
       </c>
-      <c r="O20" s="399"/>
-      <c r="P20" s="399"/>
+      <c r="O20" s="384"/>
+      <c r="P20" s="384"/>
       <c r="Q20" s="187"/>
       <c r="R20" s="189"/>
       <c r="S20" s="76"/>
@@ -10038,8 +10124,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="400"/>
-      <c r="P21" s="400"/>
+      <c r="O21" s="385"/>
+      <c r="P21" s="385"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -10151,8 +10237,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="402"/>
-      <c r="P24" s="402"/>
+      <c r="O24" s="387"/>
+      <c r="P24" s="387"/>
       <c r="Q24" s="187"/>
       <c r="R24" s="185"/>
     </row>
@@ -10613,10 +10699,10 @@
     <row r="37" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="394" t="s">
+      <c r="F37" s="379" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="394"/>
+      <c r="G37" s="379"/>
       <c r="H37" s="129">
         <f>SUM(H5:H29)</f>
         <v>41344.509999999995</v>
@@ -10655,7 +10741,7 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:18" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="404" t="s">
+      <c r="B40" s="410" t="s">
         <v>58</v>
       </c>
       <c r="C40" s="254" t="s">
@@ -10676,7 +10762,7 @@
       <c r="N40" s="212"/>
     </row>
     <row r="41" spans="2:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="404"/>
+      <c r="B41" s="410"/>
       <c r="C41" s="291" t="s">
         <v>48</v>
       </c>
@@ -10695,7 +10781,7 @@
       <c r="N41" s="212"/>
     </row>
     <row r="42" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="404"/>
+      <c r="B42" s="410"/>
       <c r="C42" s="281" t="s">
         <v>48</v>
       </c>
@@ -10718,16 +10804,16 @@
       <c r="C43" s="287" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="405" t="s">
+      <c r="D43" s="411" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="406"/>
-      <c r="F43" s="406"/>
-      <c r="G43" s="406"/>
-      <c r="H43" s="406"/>
-      <c r="I43" s="406"/>
-      <c r="J43" s="406"/>
-      <c r="K43" s="407"/>
+      <c r="E43" s="412"/>
+      <c r="F43" s="412"/>
+      <c r="G43" s="412"/>
+      <c r="H43" s="412"/>
+      <c r="I43" s="412"/>
+      <c r="J43" s="412"/>
+      <c r="K43" s="413"/>
       <c r="L43" s="206"/>
       <c r="M43" s="211"/>
       <c r="N43" s="212"/>
@@ -10735,14 +10821,14 @@
     <row r="44" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="244"/>
       <c r="C44" s="204"/>
-      <c r="D44" s="408"/>
-      <c r="E44" s="409"/>
-      <c r="F44" s="409"/>
-      <c r="G44" s="409"/>
-      <c r="H44" s="409"/>
-      <c r="I44" s="409"/>
-      <c r="J44" s="409"/>
-      <c r="K44" s="410"/>
+      <c r="D44" s="414"/>
+      <c r="E44" s="415"/>
+      <c r="F44" s="415"/>
+      <c r="G44" s="415"/>
+      <c r="H44" s="415"/>
+      <c r="I44" s="415"/>
+      <c r="J44" s="415"/>
+      <c r="K44" s="416"/>
       <c r="L44" s="206"/>
       <c r="M44" s="207"/>
       <c r="N44" s="208"/>
@@ -10782,6 +10868,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D43:K44"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="F37:G37"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -10795,14 +10889,6 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O8:P8"/>
-    <mergeCell ref="D43:K44"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="F37:G37"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.11811023622047245" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
@@ -10818,7 +10904,7 @@
   <dimension ref="B1:X47"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10843,10 +10929,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="374" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="374"/>
+      <c r="B1" s="390" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="390"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -10858,50 +10944,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="375">
+      <c r="B2" s="391">
         <v>44745</v>
       </c>
-      <c r="C2" s="376"/>
-      <c r="F2" s="377" t="s">
+      <c r="C2" s="392"/>
+      <c r="F2" s="393" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="377"/>
-      <c r="H2" s="377"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="392" t="s">
+      <c r="K2" s="408" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="392"/>
+      <c r="L2" s="408"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="378" t="s">
+      <c r="C3" s="394" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="379"/>
+      <c r="D3" s="395"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="380" t="s">
+      <c r="F3" s="396" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="381"/>
+      <c r="G3" s="397"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="382" t="s">
+      <c r="I3" s="398" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="392"/>
-      <c r="L3" s="392"/>
-      <c r="M3" s="384" t="s">
+      <c r="K3" s="408"/>
+      <c r="L3" s="408"/>
+      <c r="M3" s="400" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="385"/>
-      <c r="O3" s="386" t="s">
+      <c r="N3" s="401"/>
+      <c r="O3" s="402" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="387"/>
+      <c r="P3" s="403"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -10923,7 +11009,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="383"/>
+      <c r="I4" s="399"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -10980,8 +11066,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
-      <c r="P5" s="389"/>
+      <c r="O5" s="404"/>
+      <c r="P5" s="405"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -11019,8 +11105,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O6" s="390"/>
-      <c r="P6" s="391"/>
+      <c r="O6" s="406"/>
+      <c r="P6" s="407"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -11105,8 +11191,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O8" s="372"/>
-      <c r="P8" s="372"/>
+      <c r="O8" s="388"/>
+      <c r="P8" s="388"/>
       <c r="Q8" s="300"/>
       <c r="R8" s="185"/>
     </row>
@@ -11192,8 +11278,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="395"/>
-      <c r="P10" s="395"/>
+      <c r="O10" s="380"/>
+      <c r="P10" s="380"/>
       <c r="Q10" s="300"/>
       <c r="R10" s="185"/>
     </row>
@@ -11317,8 +11403,8 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="O13" s="397"/>
-      <c r="P13" s="397"/>
+      <c r="O13" s="382"/>
+      <c r="P13" s="382"/>
       <c r="Q13" s="331" t="s">
         <v>91</v>
       </c>
@@ -11526,8 +11612,8 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O18" s="398"/>
-      <c r="P18" s="398"/>
+      <c r="O18" s="383"/>
+      <c r="P18" s="383"/>
       <c r="Q18" s="333" t="s">
         <v>92</v>
       </c>
@@ -11614,8 +11700,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O20" s="416"/>
-      <c r="P20" s="416"/>
+      <c r="O20" s="422"/>
+      <c r="P20" s="422"/>
       <c r="Q20" s="308" t="s">
         <v>89</v>
       </c>
@@ -11651,8 +11737,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O21" s="400"/>
-      <c r="P21" s="400"/>
+      <c r="O21" s="385"/>
+      <c r="P21" s="385"/>
       <c r="Q21" s="187"/>
       <c r="R21" s="185"/>
       <c r="S21" s="53"/>
@@ -11760,8 +11846,8 @@
         <f t="shared" si="3"/>
         <v>-81</v>
       </c>
-      <c r="O24" s="402"/>
-      <c r="P24" s="402"/>
+      <c r="O24" s="387"/>
+      <c r="P24" s="387"/>
       <c r="Q24" s="334" t="s">
         <v>90</v>
       </c>
@@ -12213,10 +12299,10 @@
     <row r="37" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="126"/>
       <c r="D37" s="128"/>
-      <c r="F37" s="394" t="s">
+      <c r="F37" s="379" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="394"/>
+      <c r="G37" s="379"/>
       <c r="H37" s="129">
         <f>SUM(H5:H29)</f>
         <v>34604.840000000004</v>
@@ -12255,10 +12341,10 @@
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="2:18" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="413" t="s">
+      <c r="B40" s="419" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="357" t="s">
+      <c r="C40" s="356" t="s">
         <v>47</v>
       </c>
       <c r="D40" s="305" t="s">
@@ -12276,27 +12362,27 @@
       <c r="N40" s="212"/>
     </row>
     <row r="41" spans="2:18" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="414"/>
-      <c r="C41" s="358" t="s">
+      <c r="B41" s="420"/>
+      <c r="C41" s="357" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="411" t="s">
+      <c r="D41" s="417" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="411"/>
-      <c r="F41" s="411"/>
-      <c r="G41" s="411"/>
-      <c r="H41" s="411"/>
-      <c r="I41" s="411"/>
-      <c r="J41" s="411"/>
-      <c r="K41" s="411"/>
-      <c r="L41" s="411"/>
+      <c r="E41" s="417"/>
+      <c r="F41" s="417"/>
+      <c r="G41" s="417"/>
+      <c r="H41" s="417"/>
+      <c r="I41" s="417"/>
+      <c r="J41" s="417"/>
+      <c r="K41" s="417"/>
+      <c r="L41" s="417"/>
       <c r="M41" s="211"/>
       <c r="N41" s="212"/>
     </row>
     <row r="42" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="414"/>
-      <c r="C42" s="359" t="s">
+      <c r="B42" s="420"/>
+      <c r="C42" s="358" t="s">
         <v>49</v>
       </c>
       <c r="D42" s="296"/>
@@ -12314,30 +12400,30 @@
       <c r="N42" s="212"/>
     </row>
     <row r="43" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="414"/>
-      <c r="C43" s="360" t="s">
+      <c r="B43" s="420"/>
+      <c r="C43" s="359" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="412" t="s">
+      <c r="D43" s="418" t="s">
         <v>88</v>
       </c>
-      <c r="E43" s="412"/>
-      <c r="F43" s="412"/>
-      <c r="G43" s="412"/>
-      <c r="H43" s="412"/>
-      <c r="I43" s="412"/>
-      <c r="J43" s="412"/>
-      <c r="K43" s="412"/>
-      <c r="L43" s="412"/>
+      <c r="E43" s="418"/>
+      <c r="F43" s="418"/>
+      <c r="G43" s="418"/>
+      <c r="H43" s="418"/>
+      <c r="I43" s="418"/>
+      <c r="J43" s="418"/>
+      <c r="K43" s="418"/>
+      <c r="L43" s="418"/>
       <c r="M43" s="211"/>
       <c r="N43" s="212"/>
     </row>
     <row r="44" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="414"/>
-      <c r="C44" s="361" t="s">
+      <c r="B44" s="420"/>
+      <c r="C44" s="360" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="356" t="s">
+      <c r="D44" s="355" t="s">
         <v>110</v>
       </c>
       <c r="E44" s="326"/>
@@ -12352,12 +12438,12 @@
       <c r="N44" s="208"/>
     </row>
     <row r="45" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="414"/>
-      <c r="C45" s="362" t="s">
+      <c r="B45" s="420"/>
+      <c r="C45" s="361" t="s">
         <v>54</v>
       </c>
       <c r="D45" s="338" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E45" s="317"/>
       <c r="F45" s="317"/>
@@ -12367,15 +12453,15 @@
       <c r="J45" s="317"/>
       <c r="K45" s="317"/>
       <c r="L45" s="339"/>
-      <c r="M45" s="419"/>
-      <c r="N45" s="420"/>
-      <c r="O45" s="421"/>
-      <c r="P45" s="422"/>
-      <c r="Q45" s="423"/>
+      <c r="M45" s="372"/>
+      <c r="N45" s="373"/>
+      <c r="O45" s="374"/>
+      <c r="P45" s="375"/>
+      <c r="Q45" s="376"/>
     </row>
     <row r="46" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="414"/>
-      <c r="C46" s="363" t="s">
+      <c r="B46" s="420"/>
+      <c r="C46" s="362" t="s">
         <v>94</v>
       </c>
       <c r="D46" s="341" t="s">
@@ -12393,11 +12479,11 @@
       <c r="N46" s="208"/>
     </row>
     <row r="47" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="415"/>
-      <c r="C47" s="364" t="s">
+      <c r="B47" s="421"/>
+      <c r="C47" s="363" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="424" t="s">
+      <c r="D47" s="377" t="s">
         <v>99</v>
       </c>
       <c r="E47" s="353"/>
@@ -12414,15 +12500,6 @@
     <sortCondition ref="B5:B33"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="D41:L41"/>
-    <mergeCell ref="D43:L43"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -12436,6 +12513,15 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O8:P8"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="D41:L41"/>
+    <mergeCell ref="D43:L43"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
@@ -12450,8 +12536,8 @@
   </sheetPr>
   <dimension ref="B1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12476,10 +12562,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="B1" s="374" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="374"/>
+      <c r="B1" s="390" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="390"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -12491,50 +12577,50 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="375">
+      <c r="B2" s="391">
         <v>44773</v>
       </c>
-      <c r="C2" s="376"/>
-      <c r="F2" s="377" t="s">
+      <c r="C2" s="392"/>
+      <c r="F2" s="393" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="377"/>
-      <c r="H2" s="377"/>
+      <c r="G2" s="393"/>
+      <c r="H2" s="393"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="392" t="s">
+      <c r="K2" s="408" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="392"/>
+      <c r="L2" s="408"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
-      <c r="C3" s="378" t="s">
+      <c r="C3" s="394" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="379"/>
+      <c r="D3" s="395"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="380" t="s">
+      <c r="F3" s="396" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="381"/>
+      <c r="G3" s="397"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="382" t="s">
+      <c r="I3" s="398" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="392"/>
-      <c r="L3" s="392"/>
-      <c r="M3" s="384" t="s">
+      <c r="K3" s="408"/>
+      <c r="L3" s="408"/>
+      <c r="M3" s="400" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="385"/>
-      <c r="O3" s="386" t="s">
+      <c r="N3" s="401"/>
+      <c r="O3" s="402" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="387"/>
+      <c r="P3" s="403"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
@@ -12556,7 +12642,7 @@
       <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="383"/>
+      <c r="I4" s="399"/>
       <c r="J4" s="13"/>
       <c r="K4" s="18" t="s">
         <v>10</v>
@@ -12613,8 +12699,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
-      <c r="P5" s="389"/>
+      <c r="O5" s="404"/>
+      <c r="P5" s="405"/>
     </row>
     <row r="6" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
@@ -12652,8 +12738,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="390"/>
-      <c r="P6" s="391"/>
+      <c r="O6" s="406"/>
+      <c r="P6" s="407"/>
       <c r="S6" s="37"/>
       <c r="T6" s="38"/>
       <c r="U6" s="39"/>
@@ -12738,12 +12824,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="372"/>
-      <c r="P8" s="372"/>
+      <c r="O8" s="388"/>
+      <c r="P8" s="388"/>
       <c r="Q8" s="300"/>
       <c r="R8" s="185"/>
     </row>
-    <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:24" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B9" s="264" t="s">
         <v>16</v>
       </c>
@@ -12774,17 +12860,19 @@
       <c r="L9" s="52">
         <v>110</v>
       </c>
-      <c r="M9" s="370">
+      <c r="M9" s="369">
         <f t="shared" si="1"/>
         <v>-292.90000000000009</v>
       </c>
-      <c r="N9" s="371">
+      <c r="N9" s="370">
         <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="O9" s="48"/>
       <c r="P9" s="170"/>
-      <c r="Q9" s="187"/>
+      <c r="Q9" s="439" t="s">
+        <v>47</v>
+      </c>
       <c r="R9" s="185"/>
     </row>
     <row r="10" spans="2:24" ht="17.25" x14ac:dyDescent="0.3">
@@ -12823,9 +12911,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="395"/>
-      <c r="P10" s="395"/>
-      <c r="Q10" s="300"/>
+      <c r="O10" s="380"/>
+      <c r="P10" s="380"/>
+      <c r="Q10" s="426"/>
       <c r="R10" s="185"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" x14ac:dyDescent="0.3">
@@ -12866,11 +12954,11 @@
       </c>
       <c r="O11" s="309"/>
       <c r="P11" s="309"/>
-      <c r="Q11" s="300"/>
+      <c r="Q11" s="426"/>
       <c r="R11" s="185"/>
     </row>
     <row r="12" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="365" t="s">
+      <c r="B12" s="364" t="s">
         <v>81</v>
       </c>
       <c r="C12" s="121"/>
@@ -12907,7 +12995,7 @@
       </c>
       <c r="O12" s="61"/>
       <c r="P12" s="171"/>
-      <c r="Q12" s="300"/>
+      <c r="Q12" s="426"/>
       <c r="R12" s="185"/>
       <c r="S12" s="53"/>
       <c r="T12" s="53"/>
@@ -12948,9 +13036,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="397"/>
-      <c r="P13" s="397"/>
-      <c r="Q13" s="187"/>
+      <c r="O13" s="382"/>
+      <c r="P13" s="382"/>
+      <c r="Q13" s="190"/>
       <c r="R13" s="188"/>
       <c r="S13" s="64"/>
       <c r="T13" s="53"/>
@@ -12985,7 +13073,7 @@
       </c>
       <c r="O14" s="65"/>
       <c r="P14" s="172"/>
-      <c r="Q14" s="194"/>
+      <c r="Q14" s="190"/>
       <c r="R14" s="185"/>
       <c r="S14" s="53"/>
       <c r="T14" s="53"/>
@@ -13028,7 +13116,7 @@
       </c>
       <c r="O15" s="65"/>
       <c r="P15" s="172"/>
-      <c r="Q15" s="194"/>
+      <c r="Q15" s="190"/>
       <c r="R15" s="185"/>
       <c r="S15" s="53"/>
       <c r="T15" s="53"/>
@@ -13063,7 +13151,7 @@
       </c>
       <c r="O16" s="67"/>
       <c r="P16" s="173"/>
-      <c r="Q16" s="194"/>
+      <c r="Q16" s="190"/>
       <c r="R16" s="185"/>
       <c r="S16" s="53"/>
       <c r="T16" s="53"/>
@@ -13106,7 +13194,7 @@
       </c>
       <c r="O17" s="67"/>
       <c r="P17" s="173"/>
-      <c r="Q17" s="194"/>
+      <c r="Q17" s="190"/>
       <c r="R17" s="185"/>
       <c r="S17" s="53"/>
       <c r="T17" s="53"/>
@@ -13149,7 +13237,7 @@
       </c>
       <c r="O18" s="69"/>
       <c r="P18" s="174"/>
-      <c r="Q18" s="194"/>
+      <c r="Q18" s="190"/>
       <c r="R18" s="185"/>
       <c r="S18" s="53"/>
       <c r="T18" s="53"/>
@@ -13192,12 +13280,12 @@
       </c>
       <c r="O19" s="71"/>
       <c r="P19" s="164"/>
-      <c r="Q19" s="187"/>
+      <c r="Q19" s="190"/>
       <c r="R19" s="185"/>
       <c r="S19" s="53"/>
       <c r="T19" s="53"/>
     </row>
-    <row r="20" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="264" t="s">
         <v>25</v>
       </c>
@@ -13233,14 +13321,14 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="O20" s="398"/>
-      <c r="P20" s="398"/>
-      <c r="Q20" s="187"/>
+      <c r="O20" s="383"/>
+      <c r="P20" s="383"/>
+      <c r="Q20" s="190"/>
       <c r="R20" s="185"/>
       <c r="S20" s="53"/>
       <c r="T20" s="53"/>
     </row>
-    <row r="21" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="264" t="s">
         <v>83</v>
       </c>
@@ -13278,13 +13366,13 @@
       </c>
       <c r="O21" s="73"/>
       <c r="P21" s="175"/>
-      <c r="Q21" s="187"/>
+      <c r="Q21" s="190"/>
       <c r="R21" s="136"/>
       <c r="S21" s="75"/>
       <c r="T21" s="53"/>
     </row>
-    <row r="22" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="365" t="s">
+    <row r="22" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="364" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="25"/>
@@ -13319,14 +13407,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O22" s="399"/>
-      <c r="P22" s="399"/>
-      <c r="Q22" s="187"/>
+      <c r="O22" s="384"/>
+      <c r="P22" s="384"/>
+      <c r="Q22" s="190"/>
       <c r="R22" s="189"/>
       <c r="S22" s="76"/>
       <c r="T22" s="53"/>
     </row>
-    <row r="23" spans="2:20" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:20" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="264" t="s">
         <v>28</v>
       </c>
@@ -13354,9 +13442,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O23" s="400"/>
-      <c r="P23" s="400"/>
-      <c r="Q23" s="187"/>
+      <c r="O23" s="385"/>
+      <c r="P23" s="385"/>
+      <c r="Q23" s="190"/>
       <c r="R23" s="185"/>
       <c r="S23" s="53"/>
       <c r="T23" s="53"/>
@@ -13391,7 +13479,7 @@
       </c>
       <c r="O24" s="79"/>
       <c r="P24" s="176"/>
-      <c r="Q24" s="194"/>
+      <c r="Q24" s="190"/>
       <c r="R24" s="185"/>
     </row>
     <row r="25" spans="2:20" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -13424,10 +13512,10 @@
       </c>
       <c r="O25" s="81"/>
       <c r="P25" s="177"/>
-      <c r="Q25" s="194"/>
+      <c r="Q25" s="190"/>
       <c r="R25" s="185"/>
     </row>
-    <row r="26" spans="2:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="264" t="s">
         <v>27</v>
       </c>
@@ -13452,8 +13540,8 @@
       <c r="K26" s="83">
         <v>1983.68</v>
       </c>
-      <c r="L26" s="417">
-        <v>68</v>
+      <c r="L26" s="371">
+        <v>66</v>
       </c>
       <c r="M26" s="315">
         <f>K26-H26</f>
@@ -13461,12 +13549,12 @@
       </c>
       <c r="N26" s="290">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="402"/>
-      <c r="P26" s="402"/>
-      <c r="Q26" s="418" t="s">
-        <v>111</v>
+        <v>-2</v>
+      </c>
+      <c r="O26" s="387"/>
+      <c r="P26" s="387"/>
+      <c r="Q26" s="440" t="s">
+        <v>48</v>
       </c>
       <c r="R26" s="185"/>
     </row>
@@ -13512,11 +13600,13 @@
       </c>
       <c r="O27" s="221"/>
       <c r="P27" s="222"/>
-      <c r="Q27" s="190"/>
+      <c r="Q27" s="441" t="s">
+        <v>49</v>
+      </c>
       <c r="R27" s="185"/>
     </row>
     <row r="28" spans="2:20" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="365" t="s">
+      <c r="B28" s="364" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="25"/>
@@ -13545,10 +13635,10 @@
       </c>
       <c r="O28" s="223"/>
       <c r="P28" s="224"/>
-      <c r="Q28" s="194"/>
+      <c r="Q28" s="190"/>
       <c r="R28" s="185"/>
     </row>
-    <row r="29" spans="2:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="264" t="s">
         <v>37</v>
       </c>
@@ -13572,17 +13662,19 @@
       <c r="J29" s="31"/>
       <c r="K29" s="83"/>
       <c r="L29" s="52"/>
-      <c r="M29" s="191">
+      <c r="M29" s="443">
         <f t="shared" si="10"/>
         <v>-15457.6</v>
       </c>
-      <c r="N29" s="270">
+      <c r="N29" s="444">
         <f t="shared" si="10"/>
         <v>-17</v>
       </c>
       <c r="O29" s="223"/>
       <c r="P29" s="224"/>
-      <c r="Q29" s="225"/>
+      <c r="Q29" s="442" t="s">
+        <v>50</v>
+      </c>
       <c r="R29" s="185"/>
       <c r="S29" s="53"/>
     </row>
@@ -13610,21 +13702,21 @@
       <c r="J30" s="31"/>
       <c r="K30" s="83"/>
       <c r="L30" s="52"/>
-      <c r="M30" s="191">
+      <c r="M30" s="144">
         <f t="shared" si="10"/>
         <v>-2060</v>
       </c>
-      <c r="N30" s="270">
+      <c r="N30" s="316">
         <f t="shared" si="10"/>
         <v>-2</v>
       </c>
-      <c r="O30" s="226"/>
-      <c r="P30" s="227"/>
-      <c r="Q30" s="194"/>
-      <c r="R30" s="185"/>
+      <c r="O30" s="423"/>
+      <c r="P30" s="424"/>
+      <c r="Q30" s="425"/>
+      <c r="R30" s="317"/>
     </row>
     <row r="31" spans="2:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="366" t="s">
+      <c r="B31" s="365" t="s">
         <v>73</v>
       </c>
       <c r="C31" s="96">
@@ -13651,7 +13743,7 @@
       <c r="L31" s="52">
         <v>1</v>
       </c>
-      <c r="M31" s="191">
+      <c r="M31" s="42">
         <f t="shared" si="10"/>
         <v>0.22999999999999687</v>
       </c>
@@ -13665,7 +13757,7 @@
       <c r="R31" s="185"/>
     </row>
     <row r="32" spans="2:20" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="367" t="s">
+      <c r="B32" s="366" t="s">
         <v>96</v>
       </c>
       <c r="C32" s="96"/>
@@ -13684,7 +13776,7 @@
       <c r="J32" s="31"/>
       <c r="K32" s="83"/>
       <c r="L32" s="52"/>
-      <c r="M32" s="191">
+      <c r="M32" s="42">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13692,8 +13784,8 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O32" s="368"/>
-      <c r="P32" s="369"/>
+      <c r="O32" s="367"/>
+      <c r="P32" s="368"/>
       <c r="Q32" s="190"/>
       <c r="R32" s="185"/>
     </row>
@@ -13717,7 +13809,7 @@
       <c r="J33" s="31"/>
       <c r="K33" s="83"/>
       <c r="L33" s="52"/>
-      <c r="M33" s="191">
+      <c r="M33" s="42">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13758,7 +13850,7 @@
       <c r="L34" s="52">
         <v>50</v>
       </c>
-      <c r="M34" s="191">
+      <c r="M34" s="42">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13799,7 +13891,7 @@
       <c r="L35" s="52">
         <v>12</v>
       </c>
-      <c r="M35" s="191">
+      <c r="M35" s="42">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13844,7 +13936,7 @@
       <c r="L36" s="52">
         <v>24</v>
       </c>
-      <c r="M36" s="191">
+      <c r="M36" s="42">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13865,14 +13957,14 @@
       <c r="D37" s="26"/>
       <c r="E37" s="113"/>
       <c r="F37" s="96">
-        <v>950.75</v>
+        <v>793.09</v>
       </c>
       <c r="G37" s="106">
         <v>28</v>
       </c>
       <c r="H37" s="100">
         <f t="shared" ref="H37:I38" si="11">F37+C37</f>
-        <v>950.75</v>
+        <v>793.09</v>
       </c>
       <c r="I37" s="101">
         <f t="shared" si="11"/>
@@ -13887,7 +13979,7 @@
       </c>
       <c r="M37" s="42">
         <f t="shared" si="10"/>
-        <v>-157.64999999999998</v>
+        <v>9.9999999999909051E-3</v>
       </c>
       <c r="N37" s="43">
         <f t="shared" si="10"/>
@@ -13934,10 +14026,10 @@
     <row r="39" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="126"/>
       <c r="D39" s="128"/>
-      <c r="F39" s="394" t="s">
+      <c r="F39" s="379" t="s">
         <v>43</v>
       </c>
-      <c r="G39" s="394"/>
+      <c r="G39" s="379"/>
       <c r="H39" s="129">
         <f>SUM(H5:H31)</f>
         <v>66081.820000000007</v>
@@ -13976,13 +14068,15 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="2:18" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="413" t="s">
+      <c r="B42" s="419" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="357" t="s">
+      <c r="C42" s="356" t="s">
         <v>47</v>
       </c>
-      <c r="D42" s="305"/>
+      <c r="D42" s="305" t="s">
+        <v>112</v>
+      </c>
       <c r="E42" s="301"/>
       <c r="F42" s="301"/>
       <c r="G42" s="302"/>
@@ -13995,28 +14089,32 @@
       <c r="N42" s="212"/>
     </row>
     <row r="43" spans="2:18" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="414"/>
-      <c r="C43" s="358" t="s">
+      <c r="B43" s="420"/>
+      <c r="C43" s="357" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="411"/>
-      <c r="E43" s="411"/>
-      <c r="F43" s="411"/>
-      <c r="G43" s="411"/>
-      <c r="H43" s="411"/>
-      <c r="I43" s="411"/>
-      <c r="J43" s="411"/>
-      <c r="K43" s="411"/>
-      <c r="L43" s="411"/>
+      <c r="D43" s="427" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="427"/>
+      <c r="F43" s="427"/>
+      <c r="G43" s="427"/>
+      <c r="H43" s="427"/>
+      <c r="I43" s="427"/>
+      <c r="J43" s="427"/>
+      <c r="K43" s="427"/>
+      <c r="L43" s="427"/>
       <c r="M43" s="211"/>
       <c r="N43" s="212"/>
     </row>
     <row r="44" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="414"/>
-      <c r="C44" s="359" t="s">
+      <c r="B44" s="420"/>
+      <c r="C44" s="358" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="296"/>
+      <c r="D44" s="296" t="s">
+        <v>113</v>
+      </c>
       <c r="E44" s="297"/>
       <c r="F44" s="297"/>
       <c r="G44" s="298"/>
@@ -14029,99 +14127,84 @@
       <c r="N44" s="212"/>
     </row>
     <row r="45" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="414"/>
-      <c r="C45" s="360" t="s">
+      <c r="B45" s="420"/>
+      <c r="C45" s="431" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="412"/>
-      <c r="E45" s="412"/>
-      <c r="F45" s="412"/>
-      <c r="G45" s="412"/>
-      <c r="H45" s="412"/>
-      <c r="I45" s="412"/>
-      <c r="J45" s="412"/>
-      <c r="K45" s="412"/>
-      <c r="L45" s="412"/>
+      <c r="D45" s="428" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="428"/>
+      <c r="F45" s="428"/>
+      <c r="G45" s="428"/>
+      <c r="H45" s="428"/>
+      <c r="I45" s="428"/>
+      <c r="J45" s="428"/>
+      <c r="K45" s="428"/>
+      <c r="L45" s="428"/>
       <c r="M45" s="211"/>
       <c r="N45" s="212"/>
     </row>
     <row r="46" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="414"/>
-      <c r="C46" s="361" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="356"/>
-      <c r="E46" s="326"/>
-      <c r="F46" s="326"/>
-      <c r="G46" s="326"/>
-      <c r="H46" s="326"/>
-      <c r="I46" s="326"/>
-      <c r="J46" s="326"/>
-      <c r="K46" s="327"/>
-      <c r="L46" s="328"/>
+      <c r="B46" s="429"/>
+      <c r="C46" s="432"/>
+      <c r="D46" s="433"/>
+      <c r="E46" s="434"/>
+      <c r="F46" s="434"/>
+      <c r="G46" s="434"/>
+      <c r="H46" s="434"/>
+      <c r="I46" s="434"/>
+      <c r="J46" s="434"/>
+      <c r="K46" s="434"/>
+      <c r="L46" s="435"/>
       <c r="M46" s="207"/>
       <c r="N46" s="208"/>
     </row>
     <row r="47" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="414"/>
-      <c r="C47" s="362" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="338"/>
-      <c r="E47" s="317"/>
-      <c r="F47" s="317"/>
-      <c r="G47" s="317"/>
-      <c r="H47" s="317"/>
-      <c r="I47" s="317"/>
-      <c r="J47" s="317"/>
-      <c r="K47" s="317"/>
-      <c r="L47" s="339"/>
+      <c r="B47" s="429"/>
+      <c r="C47" s="432"/>
+      <c r="D47" s="436"/>
+      <c r="E47" s="437"/>
+      <c r="F47" s="437"/>
+      <c r="G47" s="437"/>
+      <c r="H47" s="437"/>
+      <c r="I47" s="437"/>
+      <c r="J47" s="437"/>
+      <c r="K47" s="437"/>
+      <c r="L47" s="435"/>
       <c r="M47" s="207"/>
       <c r="N47" s="208"/>
     </row>
     <row r="48" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="414"/>
-      <c r="C48" s="363" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="341"/>
-      <c r="E48" s="342"/>
-      <c r="F48" s="342"/>
-      <c r="G48" s="342"/>
-      <c r="H48" s="342"/>
-      <c r="I48" s="342"/>
-      <c r="J48" s="342"/>
-      <c r="K48" s="342"/>
-      <c r="L48" s="343"/>
+      <c r="B48" s="429"/>
+      <c r="C48" s="432"/>
+      <c r="D48" s="156"/>
+      <c r="E48" s="437"/>
+      <c r="F48" s="437"/>
+      <c r="G48" s="437"/>
+      <c r="H48" s="437"/>
+      <c r="I48" s="437"/>
+      <c r="J48" s="437"/>
+      <c r="K48" s="437"/>
+      <c r="L48" s="435"/>
       <c r="M48" s="207"/>
       <c r="N48" s="208"/>
     </row>
     <row r="49" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="415"/>
-      <c r="C49" s="364" t="s">
-        <v>98</v>
-      </c>
-      <c r="D49" s="355"/>
-      <c r="E49" s="353"/>
-      <c r="F49" s="353"/>
-      <c r="G49" s="353"/>
-      <c r="H49" s="353"/>
-      <c r="I49" s="353"/>
-      <c r="J49" s="353"/>
-      <c r="K49" s="353"/>
-      <c r="L49" s="354"/>
+      <c r="B49" s="430"/>
+      <c r="C49" s="432"/>
+      <c r="D49" s="438"/>
+      <c r="E49" s="437"/>
+      <c r="F49" s="437"/>
+      <c r="G49" s="437"/>
+      <c r="H49" s="437"/>
+      <c r="I49" s="437"/>
+      <c r="J49" s="437"/>
+      <c r="K49" s="437"/>
+      <c r="L49" s="435"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B42:B49"/>
-    <mergeCell ref="D43:L43"/>
-    <mergeCell ref="D45:L45"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F39:G39"/>
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -14135,9 +14218,18 @@
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B42:B49"/>
+    <mergeCell ref="D43:L43"/>
+    <mergeCell ref="D45:L45"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F39:G39"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="75" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>